<commit_message>
today my new commit
</commit_message>
<xml_diff>
--- a/Dominous/src/test/resources/data/inputData.xlsx
+++ b/Dominous/src/test/resources/data/inputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="8370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidData" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>DellLaptopProduct</t>
+  </si>
+  <si>
+    <t>ApplelaptopProduct</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,6 +565,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>